<commit_message>
Fixed cython errors in calc_cum_demand functions
</commit_message>
<xml_diff>
--- a/Notes/Run_time_profiling.xlsx
+++ b/Notes/Run_time_profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d992c3512c4cd48b/Documents/GitHub/DSS-Main/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A780E24C-61FA-43B2-BD1F-D0D9C2CF5D2C}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F955ED-1AD9-4C11-B9D5-0AF60A27AA2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>Mumford_0</t>
   </si>
@@ -85,12 +85,24 @@
   </si>
   <si>
     <t>G_5_P_50_R_1</t>
+  </si>
+  <si>
+    <t>G_20_P_50_R_1</t>
+  </si>
+  <si>
+    <t>Aragorn (fw_spm_cy_funcs)</t>
+  </si>
+  <si>
+    <t>G_200_P_200_R_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,10 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +436,10 @@
     <col min="3" max="3" width="1.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -478,252 +494,352 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>8</v>
+      <c r="D12" s="3">
+        <f>TIME(0,0,0.3)</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D13" s="3">
+        <f>TIME(0,0,5)</f>
+        <v>5.7870370370370366E-5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.7870370370370366E-5</v>
+      </c>
+      <c r="E14">
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.3148148148148147E-5</v>
+      </c>
+      <c r="E15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D16" s="1">
+        <v>2.3148148148148147E-5</v>
+      </c>
+      <c r="E16">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <f>SUM(D12:D16)</f>
+        <v>1.6203703703703703E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="E21">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="E24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D29" s="1">
         <v>9.0856481481481474E-5</v>
       </c>
-      <c r="E25">
+      <c r="E29">
         <v>2000</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F29" s="1">
         <v>8.1018518518518516E-5</v>
       </c>
-      <c r="G25">
+      <c r="G29">
         <v>2000</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="I29">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D30" s="1">
         <v>6.2268518518518515E-3</v>
       </c>
-      <c r="E26">
+      <c r="E30">
         <v>230000</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F30" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="G26">
+      <c r="G30">
         <v>230000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D31" s="1">
         <v>7.4074074074074068E-3</v>
       </c>
-      <c r="E27">
+      <c r="E31">
         <v>160000000</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F31" s="1">
         <v>2.7199074074074074E-3</v>
       </c>
-      <c r="G27">
+      <c r="G31">
         <v>51000000</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D32" s="1">
         <v>9.2592592592592605E-3</v>
       </c>
-      <c r="E28">
+      <c r="E32">
         <v>2000</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F32" s="1">
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="G28">
+      <c r="G32">
         <v>2000</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="I32">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D33" s="1">
         <v>1.1574074074074073E-3</v>
       </c>
-      <c r="E29">
+      <c r="E33">
         <v>243000</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F33" s="1">
         <v>9.2592592592592585E-4</v>
       </c>
-      <c r="G29">
+      <c r="G33">
         <v>2900000</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="2">
-        <f>SUM(D25:D29)</f>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f>SUM(D29:D33)</f>
         <v>2.4141782407407407E-2</v>
       </c>
-      <c r="F30" s="2">
-        <f>SUM(F25:F29)</f>
+      <c r="F34" s="2">
+        <f>SUM(F29:F33)</f>
         <v>1.4143518518518519E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D38" s="1">
         <v>2.6620370370370374E-3</v>
       </c>
-      <c r="E34">
+      <c r="E38">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D39" s="1">
         <v>1.0416666666666667E-3</v>
       </c>
-      <c r="E35">
+      <c r="E39">
         <v>22000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D40" s="1">
         <v>1.1574074074074073E-3</v>
       </c>
-      <c r="E36">
+      <c r="E40">
         <v>20000000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D41" s="1">
         <v>2.5925925925925925E-3</v>
       </c>
-      <c r="E37">
+      <c r="E41">
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D42" s="1">
         <v>1.0416666666666667E-4</v>
       </c>
-      <c r="E38">
+      <c r="E42">
         <v>24000</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="2">
-        <f>SUM(D34:D38)</f>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f>SUM(D38:D42)</f>
         <v>7.5578703703703702E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D25:D29">
+  <conditionalFormatting sqref="D29:D33">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E33 E38:E42 G29:G33">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D42">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -735,7 +851,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E29 E34:E38 G25:G29">
+  <conditionalFormatting sqref="G29:G33">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -747,7 +863,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D38">
+  <conditionalFormatting sqref="E38:E42">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -759,7 +875,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G25:G29">
+  <conditionalFormatting sqref="F29:F33">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -771,8 +897,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34:E38">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D12:D16">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -783,17 +909,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F29">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="E12:E16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Commented out main and long taking mutations
</commit_message>
<xml_diff>
--- a/Notes/Run_time_profiling.xlsx
+++ b/Notes/Run_time_profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d992c3512c4cd48b/Documents/GitHub/DSS-Main/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F955ED-1AD9-4C11-B9D5-0AF60A27AA2A}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC81924-EE53-4405-B211-BBD85031E528}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +426,7 @@
   <dimension ref="A2:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +586,9 @@
       <c r="B21" t="s">
         <v>6</v>
       </c>
+      <c r="D21" s="1">
+        <v>1.1574074074074073E-5</v>
+      </c>
       <c r="E21">
         <v>2000</v>
       </c>
@@ -599,11 +602,20 @@
       <c r="B23" t="s">
         <v>8</v>
       </c>
+      <c r="D23" s="1">
+        <v>5.3240740740740744E-4</v>
+      </c>
+      <c r="E23">
+        <v>9000000</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>9</v>
       </c>
+      <c r="D24" s="1">
+        <v>2.6620370370370372E-4</v>
+      </c>
       <c r="E24">
         <v>2000</v>
       </c>
@@ -611,6 +623,12 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>10</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.7777777777777778E-4</v>
+      </c>
+      <c r="E25">
+        <v>400000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Testing parallel Floyd Warshall
</commit_message>
<xml_diff>
--- a/Notes/Run_time_profiling.xlsx
+++ b/Notes/Run_time_profiling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d992c3512c4cd48b/Documents/GitHub/DSS-Main/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC81924-EE53-4405-B211-BBD85031E528}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="11_F25DC773A252ABDACC10488A519B4F0A5BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EECD9F3-973D-42E7-BD16-598208AE67E3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Mumford_0</t>
   </si>
@@ -93,15 +93,28 @@
     <t>Aragorn (fw_spm_cy_funcs)</t>
   </si>
   <si>
-    <t>G_200_P_200_R_1</t>
+    <t>Aragorn (fw_spm_cy_funcs) only add and remove vertex and intertwine mutations</t>
+  </si>
+  <si>
+    <t>G_1000_P_400_R_1</t>
+  </si>
+  <si>
+    <t>calc_route_set_diversity: intersection</t>
+  </si>
+  <si>
+    <t>expandTravelMatrix</t>
+  </si>
+  <si>
+    <t>DURATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -138,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I43"/>
+  <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,280 +574,459 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <f>SUM(D12:D16)</f>
         <v>1.6203703703703703E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
         <v>1.1574074074074073E-5</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>2000</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="F22" s="1">
+        <v>1.5277777777777779E-3</v>
+      </c>
+      <c r="G22">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <v>5.3240740740740744E-4</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>9000000</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F24" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G24">
+        <v>497000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>2.6620370370370372E-4</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>2000</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="F25" s="1">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="G25">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>2.7777777777777778E-4</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>400000</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="1">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G27">
+        <v>138000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="F28" s="1">
+        <v>1.1180555555555556E-2</v>
+      </c>
+      <c r="G28">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F33" t="s">
         <v>15</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D35" s="1">
         <v>9.0856481481481474E-5</v>
       </c>
-      <c r="E29">
+      <c r="E35">
         <v>2000</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F35" s="1">
         <v>8.1018518518518516E-5</v>
       </c>
-      <c r="G29">
+      <c r="G35">
         <v>2000</v>
       </c>
-      <c r="I29">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="H35" s="1">
+        <v>8.1018518518518516E-5</v>
+      </c>
+      <c r="I35">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D36" s="1">
         <v>6.2268518518518515E-3</v>
       </c>
-      <c r="E30">
+      <c r="E36">
         <v>230000</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F36" s="1">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="G30">
+      <c r="G36">
         <v>230000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D37" s="1">
         <v>7.4074074074074068E-3</v>
       </c>
-      <c r="E31">
+      <c r="E37">
         <v>160000000</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F37" s="1">
         <v>2.7199074074074074E-3</v>
       </c>
-      <c r="G31">
+      <c r="G37">
         <v>51000000</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="H37" s="1">
+        <v>3.2407407407407406E-4</v>
+      </c>
+      <c r="I37">
+        <v>8400000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D38" s="1">
         <v>9.2592592592592605E-3</v>
       </c>
-      <c r="E32">
+      <c r="E38">
         <v>2000</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F38" s="1">
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="G32">
+      <c r="G38">
         <v>2000</v>
       </c>
-      <c r="I32">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="H38" s="1">
+        <v>7.8703703703703713E-3</v>
+      </c>
+      <c r="I38">
+        <v>2000</v>
+      </c>
+      <c r="K38" s="4"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D39" s="1">
         <v>1.1574074074074073E-3</v>
       </c>
-      <c r="E33">
+      <c r="E39">
         <v>243000</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F39" s="1">
         <v>9.2592592592592585E-4</v>
       </c>
-      <c r="G33">
+      <c r="G39">
         <v>2900000</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="2">
-        <f>SUM(D29:D33)</f>
+      <c r="H39" s="1">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I39">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f>SUM(D35:D39)</f>
         <v>2.4141782407407407E-2</v>
       </c>
-      <c r="F34" s="2">
-        <f>SUM(F29:F33)</f>
+      <c r="F40" s="2">
+        <f>SUM(F35:F39)</f>
         <v>1.4143518518518519E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="H40" s="2">
+        <f>SUM(H35:H39)</f>
+        <v>9.6643518518518528E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D44" s="1">
         <v>2.6620370370370374E-3</v>
       </c>
-      <c r="E38">
+      <c r="E44">
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D45" s="1">
         <v>1.0416666666666667E-3</v>
       </c>
-      <c r="E39">
+      <c r="E45">
         <v>22000</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D46" s="1">
         <v>1.1574074074074073E-3</v>
       </c>
-      <c r="E40">
+      <c r="E46">
         <v>20000000</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D47" s="1">
         <v>2.5925925925925925E-3</v>
       </c>
-      <c r="E41">
+      <c r="E47">
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D48" s="1">
         <v>1.0416666666666667E-4</v>
       </c>
-      <c r="E42">
+      <c r="E48">
         <v>24000</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D43" s="2">
-        <f>SUM(D38:D42)</f>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f>SUM(D44:D48)</f>
         <v>7.5578703703703702E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D29:D33">
+  <conditionalFormatting sqref="D35:D39">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:E39 E44:E48 G35:G39">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44:D48">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35:G39">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:E48">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35:F39">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D16">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E16">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -845,7 +1038,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E33 E38:E42 G29:G33">
+  <conditionalFormatting sqref="H35">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -857,19 +1060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D42">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29:G33">
+  <conditionalFormatting sqref="H35:H39">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -881,7 +1072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E42">
+  <conditionalFormatting sqref="I35:I39">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -893,7 +1084,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F29:F33">
+  <conditionalFormatting sqref="D22:D26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -904,18 +1107,8 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:D16">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G28">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -927,7 +1120,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E16">
+  <conditionalFormatting sqref="E22:E26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>